<commit_message>
Changed the deleteNoneUpdateSymbols func in order to drop the ExcelWriter Object
</commit_message>
<xml_diff>
--- a/Stock_symbols_list.xlsx
+++ b/Stock_symbols_list.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SeboB\Desktop\Data Science\Foorcast\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SeboB\Desktop\Data Science\Code\FullStackTradingApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92F384CE-28CB-4608-96C8-A46E7E73F71F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4EF9BC4-7757-41A8-A3A2-B1976C7FFD93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>

<commit_message>
All Database tables implemented
</commit_message>
<xml_diff>
--- a/Stock_symbols_list.xlsx
+++ b/Stock_symbols_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SeboB\Desktop\Data Science\Code\FullStackTradingApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDE21814-359F-4B1A-9646-D3AD10697F25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F7EFEB4-FFF6-48EE-A7AC-C220EA16B13D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11760" yWindow="2700" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6840" yWindow="2160" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -20759,7 +20759,7 @@
   <dimension ref="A1:A6800"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>